<commit_message>
Update level for memo testing
</commit_message>
<xml_diff>
--- a/CenterText.xlsx
+++ b/CenterText.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\StevePro7\PlatformerSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A2A28-558B-4C46-A1AD-9281E5768946}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A074FDD2-C40D-421D-8B5B-3AAB8D1F13BF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="4020" windowWidth="16260" windowHeight="10785" xr2:uid="{F0269968-EACA-45F7-91D1-CEB5A40DA9B9}"/>
+    <workbookView xWindow="7455" yWindow="3930" windowWidth="16260" windowHeight="10785" xr2:uid="{F0269968-EACA-45F7-91D1-CEB5A40DA9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C3" si="1">IF(ISEVEN(B2),B2, B2+1)</f>
+        <f t="shared" ref="C2" si="1">IF(ISEVEN(B2),B2, B2+1)</f>
         <v>12</v>
       </c>
       <c r="D2">

</xml_diff>